<commit_message>
fixed few bugs in exporting experiment results
</commit_message>
<xml_diff>
--- a/models/dft/hecs_for_approx/parameters.xlsx
+++ b/models/dft/hecs_for_approx/parameters.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\home\thom\Documents\slurf\models\dft\hecs_for_approx\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -109,8 +114,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -173,6 +178,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -219,7 +232,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -251,9 +264,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -285,6 +299,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -460,14 +475,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -484,7 +501,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -492,16 +509,17 @@
         <v>29</v>
       </c>
       <c r="C2">
-        <v>0.0001</v>
+        <v>1E-4</v>
       </c>
       <c r="D2">
-        <v>1E-05</v>
+        <f>C2</f>
+        <v>1E-4</v>
       </c>
       <c r="E2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -509,16 +527,17 @@
         <v>29</v>
       </c>
       <c r="C3">
-        <v>0.0001</v>
+        <v>1E-4</v>
       </c>
       <c r="D3">
-        <v>1E-05</v>
+        <f t="shared" ref="D3:D25" si="0">C3</f>
+        <v>1E-4</v>
       </c>
       <c r="E3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -526,16 +545,17 @@
         <v>29</v>
       </c>
       <c r="C4">
-        <v>0.0001</v>
+        <v>1E-4</v>
       </c>
       <c r="D4">
-        <v>1E-05</v>
+        <f t="shared" si="0"/>
+        <v>1E-4</v>
       </c>
       <c r="E4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -543,16 +563,17 @@
         <v>29</v>
       </c>
       <c r="C5">
-        <v>6E-05</v>
+        <v>6.0000000000000002E-5</v>
       </c>
       <c r="D5">
-        <v>6E-06</v>
+        <f t="shared" si="0"/>
+        <v>6.0000000000000002E-5</v>
       </c>
       <c r="E5" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -560,16 +581,17 @@
         <v>29</v>
       </c>
       <c r="C6">
-        <v>6E-05</v>
+        <v>6.0000000000000002E-5</v>
       </c>
       <c r="D6">
-        <v>6E-06</v>
+        <f t="shared" si="0"/>
+        <v>6.0000000000000002E-5</v>
       </c>
       <c r="E6" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -577,16 +599,17 @@
         <v>29</v>
       </c>
       <c r="C7">
-        <v>6E-05</v>
+        <v>6.0000000000000002E-5</v>
       </c>
       <c r="D7">
-        <v>6E-06</v>
+        <f t="shared" si="0"/>
+        <v>6.0000000000000002E-5</v>
       </c>
       <c r="E7" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -594,16 +617,17 @@
         <v>29</v>
       </c>
       <c r="C8">
-        <v>6E-05</v>
+        <v>6.0000000000000002E-5</v>
       </c>
       <c r="D8">
-        <v>6E-06</v>
+        <f t="shared" si="0"/>
+        <v>6.0000000000000002E-5</v>
       </c>
       <c r="E8" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -611,16 +635,17 @@
         <v>29</v>
       </c>
       <c r="C9">
-        <v>6E-05</v>
+        <v>6.0000000000000002E-5</v>
       </c>
       <c r="D9">
-        <v>6E-06</v>
+        <f t="shared" si="0"/>
+        <v>6.0000000000000002E-5</v>
       </c>
       <c r="E9" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
@@ -628,16 +653,17 @@
         <v>29</v>
       </c>
       <c r="C10">
-        <v>1E-06</v>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="D10">
-        <v>1E-07</v>
+        <f t="shared" si="0"/>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="E10" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
@@ -645,16 +671,17 @@
         <v>29</v>
       </c>
       <c r="C11">
-        <v>1E-06</v>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="D11">
-        <v>1E-07</v>
+        <f t="shared" si="0"/>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="E11" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
@@ -662,16 +689,17 @@
         <v>29</v>
       </c>
       <c r="C12">
-        <v>5E-05</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="D12">
-        <v>5E-06</v>
+        <f t="shared" si="0"/>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="E12" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
@@ -679,16 +707,17 @@
         <v>29</v>
       </c>
       <c r="C13">
-        <v>6E-05</v>
+        <v>6.0000000000000002E-5</v>
       </c>
       <c r="D13">
-        <v>6E-06</v>
+        <f t="shared" si="0"/>
+        <v>6.0000000000000002E-5</v>
       </c>
       <c r="E13" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
@@ -696,16 +725,17 @@
         <v>29</v>
       </c>
       <c r="C14">
-        <v>0.0001</v>
+        <v>1E-4</v>
       </c>
       <c r="D14">
-        <v>1E-05</v>
+        <f t="shared" si="0"/>
+        <v>1E-4</v>
       </c>
       <c r="E14" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
@@ -713,16 +743,17 @@
         <v>29</v>
       </c>
       <c r="C15">
-        <v>0.0001</v>
+        <v>1E-4</v>
       </c>
       <c r="D15">
-        <v>1E-05</v>
+        <f t="shared" si="0"/>
+        <v>1E-4</v>
       </c>
       <c r="E15" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
@@ -730,16 +761,17 @@
         <v>29</v>
       </c>
       <c r="C16">
-        <v>0.0001</v>
+        <v>1E-4</v>
       </c>
       <c r="D16">
-        <v>1E-05</v>
+        <f t="shared" si="0"/>
+        <v>1E-4</v>
       </c>
       <c r="E16" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
@@ -747,16 +779,17 @@
         <v>29</v>
       </c>
       <c r="C17">
-        <v>6E-05</v>
+        <v>6.0000000000000002E-5</v>
       </c>
       <c r="D17">
-        <v>6E-06</v>
+        <f t="shared" si="0"/>
+        <v>6.0000000000000002E-5</v>
       </c>
       <c r="E17" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
@@ -764,16 +797,17 @@
         <v>29</v>
       </c>
       <c r="C18">
-        <v>6E-05</v>
+        <v>6.0000000000000002E-5</v>
       </c>
       <c r="D18">
-        <v>6E-06</v>
+        <f t="shared" si="0"/>
+        <v>6.0000000000000002E-5</v>
       </c>
       <c r="E18" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>22</v>
       </c>
@@ -781,16 +815,17 @@
         <v>29</v>
       </c>
       <c r="C19">
-        <v>6E-05</v>
+        <v>6.0000000000000002E-5</v>
       </c>
       <c r="D19">
-        <v>6E-06</v>
+        <f t="shared" si="0"/>
+        <v>6.0000000000000002E-5</v>
       </c>
       <c r="E19" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>23</v>
       </c>
@@ -798,16 +833,17 @@
         <v>29</v>
       </c>
       <c r="C20">
-        <v>6E-05</v>
+        <v>6.0000000000000002E-5</v>
       </c>
       <c r="D20">
-        <v>6E-06</v>
+        <f t="shared" si="0"/>
+        <v>6.0000000000000002E-5</v>
       </c>
       <c r="E20" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>24</v>
       </c>
@@ -815,16 +851,17 @@
         <v>29</v>
       </c>
       <c r="C21">
-        <v>6E-05</v>
+        <v>6.0000000000000002E-5</v>
       </c>
       <c r="D21">
-        <v>6E-06</v>
+        <f t="shared" si="0"/>
+        <v>6.0000000000000002E-5</v>
       </c>
       <c r="E21" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
@@ -832,16 +869,17 @@
         <v>29</v>
       </c>
       <c r="C22">
-        <v>1E-06</v>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="D22">
-        <v>1E-07</v>
+        <f t="shared" si="0"/>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="E22" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>26</v>
       </c>
@@ -849,16 +887,17 @@
         <v>29</v>
       </c>
       <c r="C23">
-        <v>1E-06</v>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="D23">
-        <v>1E-07</v>
+        <f t="shared" si="0"/>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="E23" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>27</v>
       </c>
@@ -866,16 +905,17 @@
         <v>29</v>
       </c>
       <c r="C24">
-        <v>5E-05</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="D24">
-        <v>5E-06</v>
+        <f t="shared" si="0"/>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="E24" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>28</v>
       </c>
@@ -883,10 +923,11 @@
         <v>29</v>
       </c>
       <c r="C25">
-        <v>6E-05</v>
+        <v>6.0000000000000002E-5</v>
       </c>
       <c r="D25">
-        <v>6E-06</v>
+        <f t="shared" si="0"/>
+        <v>6.0000000000000002E-5</v>
       </c>
       <c r="E25" t="b">
         <v>0</v>

</xml_diff>